<commit_message>
Adding files to reproduce figures and updating READMEs
</commit_message>
<xml_diff>
--- a/Synthetic Data for Regression/ParameterSets_FiniteSampSize.xlsx
+++ b/Synthetic Data for Regression/ParameterSets_FiniteSampSize.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\andrew\Projects\Indistinguishability-Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\andrew\Projects\PowerLaw\Synthetic Data for Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB07399-136A-4FD9-A7D9-FCB32291B695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52CD83D-BEBE-4D94-B246-12808C6F9D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{795F4FF9-ADD0-4357-A1B9-4961C3A47C55}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>N</t>
   </si>
@@ -95,12 +95,6 @@
   </si>
   <si>
     <t>ps number</t>
-  </si>
-  <si>
-    <t>yes: exclude 50</t>
-  </si>
-  <si>
-    <t>yes: exclude 50 &amp; 100</t>
   </si>
 </sst>
 </file>
@@ -486,26 +480,26 @@
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -564,7 +558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -623,7 +617,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -682,7 +676,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -741,7 +735,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -800,7 +794,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -859,7 +853,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -918,7 +912,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -977,7 +971,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1036,7 +1030,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1095,7 +1089,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1154,7 +1148,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1213,7 +1207,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1272,7 +1266,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1331,7 +1325,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1390,7 +1384,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1508,7 +1502,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1567,7 +1561,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1626,7 +1620,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1685,7 +1679,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1752,31 +1746,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF2B9A3-933A-4C16-BA92-B46120924DF8}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1829,13 +1822,10 @@
         <v>13</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1887,14 +1877,11 @@
       <c r="Q2" s="5">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1946,14 +1933,11 @@
       <c r="Q3" s="5">
         <v>1</v>
       </c>
-      <c r="R3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2005,14 +1989,11 @@
       <c r="Q4" s="5">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2064,14 +2045,11 @@
       <c r="Q5" s="5">
         <v>1</v>
       </c>
-      <c r="R5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2123,14 +2101,11 @@
       <c r="Q6" s="5">
         <v>1</v>
       </c>
-      <c r="R6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2182,14 +2157,11 @@
       <c r="Q7" s="5">
         <v>1</v>
       </c>
-      <c r="R7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2241,14 +2213,11 @@
       <c r="Q8" s="11">
         <v>1</v>
       </c>
-      <c r="R8" t="s">
-        <v>18</v>
-      </c>
-      <c r="S8">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2300,14 +2269,11 @@
       <c r="Q9" s="5">
         <v>1</v>
       </c>
-      <c r="R9" t="s">
-        <v>18</v>
-      </c>
-      <c r="S9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2359,14 +2325,11 @@
       <c r="Q10" s="5">
         <v>1</v>
       </c>
-      <c r="R10" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2418,14 +2381,11 @@
       <c r="Q11" s="5">
         <v>1</v>
       </c>
-      <c r="R11" t="s">
-        <v>18</v>
-      </c>
-      <c r="S11">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2477,14 +2437,11 @@
       <c r="Q12" s="5">
         <v>1</v>
       </c>
-      <c r="R12" t="s">
-        <v>18</v>
-      </c>
-      <c r="S12">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2536,14 +2493,11 @@
       <c r="Q13" s="5">
         <v>1</v>
       </c>
-      <c r="R13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S13">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2595,14 +2549,11 @@
       <c r="Q14" s="5">
         <v>1</v>
       </c>
-      <c r="R14" t="s">
-        <v>20</v>
-      </c>
-      <c r="S14">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2654,14 +2605,11 @@
       <c r="Q15" s="5">
         <v>1</v>
       </c>
-      <c r="R15" t="s">
-        <v>20</v>
-      </c>
-      <c r="S15">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2713,14 +2661,11 @@
       <c r="Q16" s="5">
         <v>1</v>
       </c>
-      <c r="R16" t="s">
-        <v>20</v>
-      </c>
-      <c r="S16">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2772,14 +2717,11 @@
       <c r="Q17" s="5">
         <v>1</v>
       </c>
-      <c r="R17" t="s">
-        <v>20</v>
-      </c>
-      <c r="S17">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2831,14 +2773,11 @@
       <c r="Q18" s="5">
         <v>1</v>
       </c>
-      <c r="R18" t="s">
-        <v>20</v>
-      </c>
-      <c r="S18">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R18">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2890,14 +2829,11 @@
       <c r="Q19" s="5">
         <v>1</v>
       </c>
-      <c r="R19" t="s">
-        <v>20</v>
-      </c>
-      <c r="S19">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2949,14 +2885,11 @@
       <c r="Q20" s="5">
         <v>1</v>
       </c>
-      <c r="R20" t="s">
-        <v>20</v>
-      </c>
-      <c r="S20">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3008,10 +2941,7 @@
       <c r="Q21" s="5">
         <v>1</v>
       </c>
-      <c r="R21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S21">
+      <c r="R21">
         <v>5000</v>
       </c>
     </row>

</xml_diff>